<commit_message>
examples and updated graphs
</commit_message>
<xml_diff>
--- a/tacc_tests/development_log_study_2.xlsx
+++ b/tacc_tests/development_log_study_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghajoshi/Box Sync/Dissertation_Joshi/simulation/tacc_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C53FAC-C680-A841-8E87-E8A461B849F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156961A6-C3F0-9941-A43E-5569A4D6D6F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{E171DE8D-CEF9-4C4E-96B4-2838716011F6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>seed_overall</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>simulation/tacc_tests/12_10/sim_test2_1.Rdata</t>
+  </si>
+  <si>
+    <t>set.seed(20201210)</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B450F53-7566-6449-A260-22D7827A0E0F}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,6 +527,33 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <f>68 * B4</f>
+        <v>204</v>
+      </c>
+      <c r="D4">
+        <v>399</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.3912037037037034E-2</v>
+      </c>
+      <c r="H4">
+        <v>1527.413</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>